<commit_message>
Se definen tareas para el primer sprint
</commit_message>
<xml_diff>
--- a/documentacion/desarrollo/Product Backlog Sibica.xlsx
+++ b/documentacion/desarrollo/Product Backlog Sibica.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUIS\Documents\sibica\documentacion\desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sibica\documentacion\desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PB" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="210">
   <si>
     <t>Enunciado de la Historia</t>
   </si>
@@ -1336,42 +1336,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Como </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>usuario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, necesito poder visualizar en añplicativo web cada polígono que representa un predio, ubicado en el mapa de Cali a partir de sus coordenadas geográficas tomadas de una Base de Datos PostgreSQL alojada en un servidor de la UAEGBS, con la finalidad de </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>visualizar geográficamente todos los predios de uso público y Fiscal en el mapa de la ciudad de Santiago de Cali.</t>
-    </r>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -2181,6 +2145,130 @@
   </si>
   <si>
     <t>SPRINT BACKLOG - SPRINT 4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Como </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, necesito poder visualizar en el aplicativo web cada polígono que representa un predio, ubicado en el mapa de Cali a partir de sus coordenadas geográficas tomadas de una Base de Datos PostgreSQL alojada en un servidor de la UAEGBS, con la finalidad de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>visualizar geográficamente todos los predios de uso público y Fiscal en el mapa de la ciudad de Santiago de Cali.</t>
+    </r>
+  </si>
+  <si>
+    <t>Como usuario, necesito que la aplicación web permita advertir que la información mostrada actualmente no corresponde a la totalidad de predios del Municipio ya que se está actualizando constantemente.</t>
+  </si>
+  <si>
+    <t>Como usuario Administrador, necesito que la aplicación web permita la creación, edición, activación e inactivación de usuarios:
+Conforme a lo expuesto en el requerimiento RF1, se requiere que la aplicación permita crear, editar, activar e inactivar a un usuario y asignarle un determinado rol, dicha información reposará en la Base de Datos de la aplicación.</t>
+  </si>
+  <si>
+    <t>Como usuario, necesito que la aplicación web permita gestionar automáticamente el cierre de cesión transcurrido cinco (5) minutos de inactividad.</t>
+  </si>
+  <si>
+    <t>Como usuario, necesito que la aplicación permita bloquear al usuario cuando tenga más de tres (3) intentos fallidos de logueo.</t>
+  </si>
+  <si>
+    <t>Como usuario, necesito que la aplicación permita mostrar u ocultar otros campos de información alfanumérica de la base de Datos y restringir su visualización por roles.</t>
+  </si>
+  <si>
+    <t>Como usuario Administrador, necesito que la aplicación permita establecer qué campos de información de la Base de Datos pueden ver cada uno de los roles creados.</t>
+  </si>
+  <si>
+    <t>Identificar el punto en donde se realiza la consulta de los predios</t>
+  </si>
+  <si>
+    <t>Generar modal emergente indicando al usuario que la informacion mostrada actualmente no corresponde a la totalidad de predios del Municipio ya que se está actualizando constantemente.</t>
+  </si>
+  <si>
+    <t>Realizar CRUD de roles</t>
+  </si>
+  <si>
+    <t>Realizar CRUD de usuarios</t>
+  </si>
+  <si>
+    <t>Realizar CRUD de de tablas</t>
+  </si>
+  <si>
+    <t>Realizar CRUD de campos</t>
+  </si>
+  <si>
+    <t>Realizar modulo para gestionar la permisoogia para roles</t>
+  </si>
+  <si>
+    <t>Realizar modulo para gestionar los roles de un usuario</t>
+  </si>
+  <si>
+    <t>Validar a que tablas y que campos de esta, tiene permisos un rol determinado</t>
+  </si>
+  <si>
+    <t>Validar la permisologia del usuario, de acuerdo a los roles que posee</t>
+  </si>
+  <si>
+    <t>T005</t>
+  </si>
+  <si>
+    <t>T006</t>
+  </si>
+  <si>
+    <t>Validar la inactividad del usuario en sesion</t>
+  </si>
+  <si>
+    <t>Cerrar session despues de trascurrido el tiempo estipulado</t>
+  </si>
+  <si>
+    <t>Como usuario Administrador, necesito que la aplicación web permita crear, editar, activar e inactivar tipos de amoblamientos y definir su icono para la representación gráfica, los cuales toma de la base de datos.</t>
+  </si>
+  <si>
+    <t>Validar la cantidad de veces que el usuario falla al iniciar sesion</t>
+  </si>
+  <si>
+    <t>Cuando los intestos fallidos lleguen a la cifra estpulada, pasar el estado del usuario, a usuario bloqueado</t>
+  </si>
+  <si>
+    <t>Realizar CRUD de para tipo de amoblamientos</t>
+  </si>
+  <si>
+    <t>Ajustar la representacion de este amoblamiento en el mapa, con base al icono definido en este</t>
+  </si>
+  <si>
+    <t>Validar a la hora de consultar, que campos puede visualizar el usuario en sesion, de acuerdo a los roles que este contenga</t>
+  </si>
+  <si>
+    <t>Mostrar al usuario solo los campos permitidos., de acuerdo a los roles que contenga.</t>
+  </si>
+  <si>
+    <t>Validar a la hora de consultar predios, que campos se encuentran con valor null</t>
+  </si>
+  <si>
+    <t>Omitir en la visualizacion aquellos campos del predio que contengan null como valor</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2416,12 +2504,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2466,6 +2563,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2499,7 +2600,45 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
@@ -2817,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="81.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2834,56 +2973,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -2919,7 +3058,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>135</v>
+        <v>180</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>113</v>
@@ -2929,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -2951,7 +3090,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2963,7 +3102,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>113</v>
@@ -2973,19 +3112,19 @@
         <v>2</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>113</v>
@@ -2995,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -3007,7 +3146,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>113</v>
@@ -3017,19 +3156,19 @@
         <v>3</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>113</v>
@@ -3039,7 +3178,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -3051,7 +3190,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>113</v>
@@ -3061,19 +3200,19 @@
         <v>2</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>113</v>
@@ -3083,7 +3222,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -3095,7 +3234,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>113</v>
@@ -3105,21 +3244,21 @@
         <v>2</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>113</v>
@@ -3129,10 +3268,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3143,7 +3282,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>113</v>
@@ -3153,10 +3292,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3167,44 +3306,44 @@
         <v>31</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1">
+      <c r="F18" s="29">
         <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="F19" s="29">
         <v>2</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3215,39 +3354,39 @@
         <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="1">
+      <c r="F20" s="29">
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1">
+      <c r="F21" s="29">
         <v>2</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -3265,17 +3404,17 @@
         <v>113</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="1">
+      <c r="F22" s="29">
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>33</v>
@@ -3287,11 +3426,11 @@
         <v>113</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="1">
+      <c r="F23" s="29">
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -3303,39 +3442,39 @@
         <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1">
+      <c r="F24" s="29">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1">
+      <c r="F25" s="29">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -3353,10 +3492,10 @@
         <v>113</v>
       </c>
       <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3373,10 +3512,10 @@
         <v>113</v>
       </c>
       <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3387,41 +3526,41 @@
         <v>38</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1">
+      <c r="F28" s="29">
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="1">
+      <c r="F29" s="29">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -3433,20 +3572,20 @@
         <v>39</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1">
+      <c r="F30" s="29">
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3457,20 +3596,20 @@
         <v>40</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="1">
+      <c r="F31" s="29">
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3481,39 +3620,39 @@
         <v>41</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="1">
+      <c r="F32" s="29">
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="1">
+      <c r="F33" s="29">
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -3531,11 +3670,11 @@
         <v>113</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="1">
+      <c r="F34" s="29">
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -3547,17 +3686,17 @@
         <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="1">
+      <c r="F35" s="29">
         <v>2</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -3575,11 +3714,11 @@
         <v>113</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1">
+      <c r="F36" s="29">
         <v>1</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -3597,11 +3736,11 @@
         <v>113</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1">
+      <c r="F37" s="29">
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -3619,11 +3758,11 @@
         <v>113</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="1">
+      <c r="F38" s="29">
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -3641,11 +3780,11 @@
         <v>113</v>
       </c>
       <c r="E39" s="1"/>
-      <c r="F39" s="1">
+      <c r="F39" s="29">
         <v>4</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H39" s="1"/>
     </row>
@@ -3663,11 +3802,11 @@
         <v>113</v>
       </c>
       <c r="E40" s="1"/>
-      <c r="F40" s="1">
+      <c r="F40" s="29">
         <v>2</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -3685,11 +3824,11 @@
         <v>113</v>
       </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1">
+      <c r="F41" s="29">
         <v>2</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -3707,11 +3846,11 @@
         <v>113</v>
       </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1">
+      <c r="F42" s="29">
         <v>2</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H42" s="1"/>
     </row>
@@ -3729,11 +3868,11 @@
         <v>113</v>
       </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="1">
+      <c r="F43" s="29">
         <v>4</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -3751,11 +3890,11 @@
         <v>113</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="1">
+      <c r="F44" s="29">
         <v>3</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -3773,14 +3912,14 @@
         <v>113</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="1">
+      <c r="F45" s="29">
         <v>3</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -3797,11 +3936,11 @@
         <v>113</v>
       </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="1">
+      <c r="F46" s="29">
         <v>3</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -3819,11 +3958,11 @@
         <v>113</v>
       </c>
       <c r="E47" s="1"/>
-      <c r="F47" s="1">
+      <c r="F47" s="29">
         <v>4</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H47" s="1"/>
     </row>
@@ -3841,11 +3980,11 @@
         <v>113</v>
       </c>
       <c r="E48" s="1"/>
-      <c r="F48" s="1">
+      <c r="F48" s="29">
         <v>4</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H48" s="1"/>
     </row>
@@ -3863,11 +4002,11 @@
         <v>113</v>
       </c>
       <c r="E49" s="1"/>
-      <c r="F49" s="1">
+      <c r="F49" s="29">
         <v>4</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -3885,11 +4024,11 @@
         <v>113</v>
       </c>
       <c r="E50" s="1"/>
-      <c r="F50" s="1">
+      <c r="F50" s="29">
         <v>4</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H50" s="1"/>
     </row>
@@ -3907,11 +4046,11 @@
         <v>113</v>
       </c>
       <c r="E51" s="1"/>
-      <c r="F51" s="1">
+      <c r="F51" s="29">
         <v>4</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H51" s="1"/>
     </row>
@@ -3929,7 +4068,7 @@
         <v>113</v>
       </c>
       <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
+      <c r="F52" s="29"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
@@ -3947,7 +4086,7 @@
         <v>113</v>
       </c>
       <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="F53" s="29"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
@@ -3965,7 +4104,7 @@
         <v>113</v>
       </c>
       <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+      <c r="F54" s="29"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
@@ -3983,7 +4122,7 @@
         <v>113</v>
       </c>
       <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+      <c r="F55" s="29"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
@@ -3992,7 +4131,7 @@
         <v>90</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>89</v>
@@ -4001,7 +4140,7 @@
         <v>113</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
+      <c r="F56" s="29"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
@@ -4033,10 +4172,1229 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84:E86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="81.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="22"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="22"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="22"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="22"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="22"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="22"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+    </row>
+    <row r="47" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="38"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="39"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="39"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="39"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="39"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+    </row>
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="22"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="22"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="22"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="24"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+    </row>
+    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+    </row>
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="22"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="22"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="22"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="24"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+    </row>
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+    </row>
+    <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="22"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="22"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="22"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="22"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="22"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="24"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+    </row>
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="20"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="22"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="22"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="22"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="22"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="22"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="24"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+    </row>
+    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="20"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" s="6"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="22"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="22"/>
+      <c r="B85" s="36"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="22"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="22"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="22"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="24"/>
+      <c r="B89" s="37"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="31"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A55:B59"/>
+    <mergeCell ref="A67:B73"/>
+    <mergeCell ref="A75:B81"/>
+    <mergeCell ref="A83:B89"/>
+    <mergeCell ref="A61:B65"/>
+    <mergeCell ref="A24:B30"/>
+    <mergeCell ref="A32:B38"/>
+    <mergeCell ref="A40:B46"/>
+    <mergeCell ref="A1:H5"/>
+    <mergeCell ref="A8:B14"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A16:B22"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="81.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4051,56 +5409,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -4128,91 +5486,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
       <c r="E12" s="6"/>
@@ -4221,8 +5547,8 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="6"/>
@@ -4231,8 +5557,8 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -4240,91 +5566,59 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>24</v>
-      </c>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="6"/>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6"/>
@@ -4333,8 +5627,8 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="6"/>
       <c r="D21" s="1"/>
       <c r="E21" s="6"/>
@@ -4343,281 +5637,8 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:H5"/>
-    <mergeCell ref="A8:B14"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A16:B22"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection sqref="A1:H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="81.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4651,56 +5672,56 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -4734,13 +5755,13 @@
       <c r="C7" s="6"/>
       <c r="D7" s="1"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="6"/>
@@ -4749,8 +5770,8 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="6"/>
       <c r="D9" s="1"/>
       <c r="E9" s="6"/>
@@ -4759,8 +5780,8 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="6"/>
       <c r="D10" s="1"/>
       <c r="E10" s="6"/>
@@ -4769,8 +5790,8 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="6"/>
       <c r="D11" s="1"/>
       <c r="E11" s="6"/>
@@ -4779,8 +5800,8 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
       <c r="E12" s="6"/>
@@ -4789,8 +5810,8 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="6"/>
@@ -4799,8 +5820,8 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -4814,13 +5835,13 @@
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="6"/>
       <c r="D16" s="1"/>
       <c r="E16" s="6"/>
@@ -4829,8 +5850,8 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="6"/>
       <c r="D17" s="1"/>
       <c r="E17" s="6"/>
@@ -4839,8 +5860,8 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="6"/>
       <c r="D18" s="1"/>
       <c r="E18" s="6"/>
@@ -4849,8 +5870,8 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="1"/>
       <c r="E19" s="6"/>
@@ -4859,8 +5880,8 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6"/>
@@ -4869,8 +5890,8 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="6"/>
       <c r="D21" s="1"/>
       <c r="E21" s="6"/>
@@ -4879,8 +5900,8 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -4904,63 +5925,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -4994,24 +6015,24 @@
       <c r="C7" s="6"/>
       <c r="D7" s="1"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="J8" s="27"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="6"/>
       <c r="D9" s="1"/>
       <c r="E9" s="6"/>
@@ -5020,8 +6041,8 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="6"/>
       <c r="D10" s="1"/>
       <c r="E10" s="6"/>
@@ -5030,8 +6051,8 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="6"/>
       <c r="D11" s="1"/>
       <c r="E11" s="6"/>
@@ -5040,8 +6061,8 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="6"/>
       <c r="D12" s="1"/>
       <c r="E12" s="6"/>
@@ -5050,8 +6071,8 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="6"/>
@@ -5060,8 +6081,8 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -5075,13 +6096,13 @@
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="6"/>
       <c r="D16" s="1"/>
       <c r="E16" s="6"/>
@@ -5090,8 +6111,8 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="6"/>
       <c r="D17" s="1"/>
       <c r="E17" s="6"/>
@@ -5100,8 +6121,8 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="6"/>
       <c r="D18" s="1"/>
       <c r="E18" s="6"/>
@@ -5110,8 +6131,8 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="1"/>
       <c r="E19" s="6"/>
@@ -5120,8 +6141,8 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="6"/>
       <c r="D20" s="1"/>
       <c r="E20" s="6"/>
@@ -5130,8 +6151,8 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="6"/>
       <c r="D21" s="1"/>
       <c r="E21" s="6"/>
@@ -5140,8 +6161,8 @@
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>

</xml_diff>